<commit_message>
Ajustes para inserir checklist
</commit_message>
<xml_diff>
--- a/src/main/resources/BancoDeDados.xlsx
+++ b/src/main/resources/BancoDeDados.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">Materiais – G</t>
+    <t xml:space="preserve">Alternador</t>
   </si>
   <si>
-    <t xml:space="preserve">Materiais – M</t>
+    <t xml:space="preserve">Airbag</t>
   </si>
   <si>
-    <t xml:space="preserve">Materiais – P</t>
+    <t xml:space="preserve">Ala do teto</t>
   </si>
 </sst>
 </file>
@@ -108,7 +108,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,7 +238,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Login Route 66 e ajustes
</commit_message>
<xml_diff>
--- a/src/main/resources/BancoDeDados.xlsx
+++ b/src/main/resources/BancoDeDados.xlsx
@@ -20,15 +20,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">Alternador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Airbag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ala do teto</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+  <si>
+    <t xml:space="preserve">Pintura: 1 Hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 1 Hora e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 2 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 2 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 3 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 3 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 4 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 4 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 5 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 5 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 6 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 6 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 7 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 7 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 8 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 8 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 9 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 9 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 10 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 10 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 11 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 11 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 12 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 12 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 13 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 13 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 14 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 14 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 15 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 15 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 16 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 16 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 17 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 17 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 18 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 18 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 19 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 19 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 20 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 20 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 21 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 21 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 22 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 22 Horas e 30 minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 23 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura: 23 Horas e 30 minutos</t>
   </si>
 </sst>
 </file>
@@ -103,8 +232,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -235,36 +368,419 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.92"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>